<commit_message>
Modified Wave5.xlsx and Wave7.xlsx for 3rd column of service provider solution listing Modified ProductLandingVariation10.java for extra comment in report
</commit_message>
<xml_diff>
--- a/docs/Language Waves/Wave5.xlsx
+++ b/docs/Language Waves/Wave5.xlsx
@@ -1705,9 +1705,6 @@
     <t>http://www.cisco.com/web/JP/solution/isp/solutions-listing.html</t>
   </si>
   <si>
-    <t>solution-listing-var9</t>
-  </si>
-  <si>
     <t>http://www.cisco.com/web/JP/solution/isp/product-listing.html</t>
   </si>
   <si>
@@ -1715,6 +1712,9 @@
   </si>
   <si>
     <t>http://www.cisco.com/cisco/web/JP/support/index.html</t>
+  </si>
+  <si>
+    <t>solutions-listing-var9</t>
   </si>
 </sst>
 </file>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
@@ -2646,7 +2646,7 @@
         <v>79</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>145</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="36" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>79</v>
@@ -6848,7 +6848,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">

</xml_diff>

<commit_message>
Added one url in ja_jp
</commit_message>
<xml_diff>
--- a/docs/Language Waves/Wave5.xlsx
+++ b/docs/Language Waves/Wave5.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration\OVWMigration\docs\Language Waves\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7152" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="7" r:id="rId1"/>
@@ -20,7 +25,7 @@
     <sheet name="sv_se" sheetId="19" r:id="rId11"/>
     <sheet name="no_no" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="560">
   <si>
     <t>http://www.cisco.com/web/JP/ordering/index.html</t>
   </si>
@@ -1704,6 +1709,12 @@
   </si>
   <si>
     <t>solutions-listing-var9</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/isp/benefit.html</t>
+  </si>
+  <si>
+    <t>benefit-var2</t>
   </si>
 </sst>
 </file>
@@ -2052,7 +2063,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2060,20 +2071,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2086,7 +2097,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2099,7 +2110,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2112,7 +2123,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2125,7 +2136,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2140,7 +2151,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2155,7 +2166,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2172,7 +2183,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2189,7 +2200,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2206,7 +2217,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2223,7 +2234,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2240,7 +2251,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -2257,7 +2268,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -2274,7 +2285,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2291,7 +2302,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -2308,7 +2319,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2325,7 +2336,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2342,7 +2353,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2359,7 +2370,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2376,7 +2387,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2393,7 +2404,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2410,7 +2421,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2427,7 +2438,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2444,7 +2455,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2461,7 +2472,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2478,7 +2489,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2495,7 +2506,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2512,7 +2523,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2527,7 +2538,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2544,7 +2555,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2561,7 +2572,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2578,7 +2589,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2595,7 +2606,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>283</v>
       </c>
@@ -2612,7 +2623,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>554</v>
       </c>
@@ -2629,7 +2640,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>555</v>
       </c>
@@ -2646,7 +2657,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
@@ -2661,7 +2672,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
@@ -2676,7 +2687,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
@@ -2693,7 +2704,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
@@ -2710,7 +2721,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
@@ -2727,7 +2738,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>285</v>
       </c>
@@ -2744,7 +2755,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
@@ -2761,7 +2772,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
@@ -2778,7 +2789,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
@@ -2795,7 +2806,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
@@ -2812,7 +2823,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>41</v>
       </c>
@@ -2829,7 +2840,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>42</v>
       </c>
@@ -2844,7 +2855,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>43</v>
       </c>
@@ -2861,7 +2872,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>44</v>
       </c>
@@ -2878,7 +2889,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>45</v>
       </c>
@@ -2895,7 +2906,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
@@ -2912,7 +2923,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>47</v>
       </c>
@@ -2929,7 +2940,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>48</v>
       </c>
@@ -2946,7 +2957,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>49</v>
       </c>
@@ -2963,7 +2974,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>50</v>
       </c>
@@ -2980,7 +2991,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
@@ -2997,7 +3008,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>52</v>
       </c>
@@ -3014,7 +3025,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>53</v>
       </c>
@@ -3031,7 +3042,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>54</v>
       </c>
@@ -3048,7 +3059,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>55</v>
       </c>
@@ -3065,7 +3076,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>56</v>
       </c>
@@ -3082,7 +3093,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>57</v>
       </c>
@@ -3099,7 +3110,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>58</v>
       </c>
@@ -3116,7 +3127,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>59</v>
       </c>
@@ -3133,7 +3144,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>60</v>
       </c>
@@ -3150,7 +3161,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>61</v>
       </c>
@@ -3167,7 +3178,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>62</v>
       </c>
@@ -3184,7 +3195,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>63</v>
       </c>
@@ -3201,7 +3212,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>64</v>
       </c>
@@ -3218,7 +3229,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>65</v>
       </c>
@@ -3235,7 +3246,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>66</v>
       </c>
@@ -3252,7 +3263,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>67</v>
       </c>
@@ -3269,7 +3280,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>68</v>
       </c>
@@ -3286,7 +3297,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>69</v>
       </c>
@@ -3303,7 +3314,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>70</v>
       </c>
@@ -3320,7 +3331,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>71</v>
       </c>
@@ -3337,7 +3348,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>72</v>
       </c>
@@ -3351,6 +3362,23 @@
         <v>147</v>
       </c>
       <c r="E77" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="B78" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" t="s">
+        <v>559</v>
+      </c>
+      <c r="D78" t="s">
+        <v>145</v>
+      </c>
+      <c r="E78" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3365,11 +3393,11 @@
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3839,11 +3867,11 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4326,11 +4354,11 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4809,18 +4837,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="91.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>148</v>
       </c>
@@ -4833,7 +4861,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>149</v>
       </c>
@@ -4846,7 +4874,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>150</v>
       </c>
@@ -4859,7 +4887,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>151</v>
       </c>
@@ -4872,7 +4900,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>152</v>
       </c>
@@ -4887,7 +4915,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>153</v>
       </c>
@@ -4902,7 +4930,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>154</v>
       </c>
@@ -4919,7 +4947,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>155</v>
       </c>
@@ -4936,7 +4964,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>156</v>
       </c>
@@ -4953,7 +4981,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>157</v>
       </c>
@@ -4970,7 +4998,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>158</v>
       </c>
@@ -4987,7 +5015,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>159</v>
       </c>
@@ -5004,7 +5032,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>160</v>
       </c>
@@ -5019,7 +5047,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>161</v>
       </c>
@@ -5036,7 +5064,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>162</v>
       </c>
@@ -5053,7 +5081,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>163</v>
       </c>
@@ -5070,7 +5098,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>164</v>
       </c>
@@ -5087,7 +5115,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>165</v>
       </c>
@@ -5102,7 +5130,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>166</v>
       </c>
@@ -5117,7 +5145,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>167</v>
       </c>
@@ -5134,7 +5162,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>168</v>
       </c>
@@ -5151,7 +5179,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>169</v>
       </c>
@@ -5168,7 +5196,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>170</v>
       </c>
@@ -5185,7 +5213,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>171</v>
       </c>
@@ -5202,7 +5230,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>172</v>
       </c>
@@ -5219,7 +5247,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>173</v>
       </c>
@@ -5236,7 +5264,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>174</v>
       </c>
@@ -5253,7 +5281,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>175</v>
       </c>
@@ -5268,7 +5296,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>176</v>
       </c>
@@ -5285,7 +5313,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>177</v>
       </c>
@@ -5302,7 +5330,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>178</v>
       </c>
@@ -5319,7 +5347,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>179</v>
       </c>
@@ -5336,7 +5364,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>180</v>
       </c>
@@ -5353,7 +5381,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>181</v>
       </c>
@@ -5370,7 +5398,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>182</v>
       </c>
@@ -5387,7 +5415,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>183</v>
       </c>
@@ -5404,7 +5432,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>184</v>
       </c>
@@ -5421,7 +5449,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>185</v>
       </c>
@@ -5438,7 +5466,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>186</v>
       </c>
@@ -5455,7 +5483,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>187</v>
       </c>
@@ -5472,7 +5500,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>188</v>
       </c>
@@ -5489,7 +5517,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>189</v>
       </c>
@@ -5506,7 +5534,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>190</v>
       </c>
@@ -5523,7 +5551,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>191</v>
       </c>
@@ -5540,7 +5568,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>192</v>
       </c>
@@ -5557,7 +5585,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>193</v>
       </c>
@@ -5574,7 +5602,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>194</v>
       </c>
@@ -5591,7 +5619,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>195</v>
       </c>
@@ -5608,7 +5636,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>196</v>
       </c>
@@ -5625,7 +5653,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>197</v>
       </c>
@@ -5642,7 +5670,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>198</v>
       </c>
@@ -5659,7 +5687,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>199</v>
       </c>
@@ -5676,7 +5704,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>200</v>
       </c>
@@ -5706,14 +5734,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="91.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>148</v>
       </c>
@@ -5724,7 +5752,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>149</v>
       </c>
@@ -5735,7 +5763,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>150</v>
       </c>
@@ -5746,7 +5774,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>151</v>
       </c>
@@ -5757,7 +5785,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>152</v>
       </c>
@@ -5771,7 +5799,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>153</v>
       </c>
@@ -5785,7 +5813,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>154</v>
       </c>
@@ -5802,7 +5830,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>155</v>
       </c>
@@ -5819,7 +5847,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>156</v>
       </c>
@@ -5836,7 +5864,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>157</v>
       </c>
@@ -5853,7 +5881,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>158</v>
       </c>
@@ -5870,7 +5898,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>159</v>
       </c>
@@ -5887,7 +5915,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>160</v>
       </c>
@@ -5901,7 +5929,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>161</v>
       </c>
@@ -5918,7 +5946,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>162</v>
       </c>
@@ -5935,7 +5963,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>163</v>
       </c>
@@ -5952,7 +5980,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>164</v>
       </c>
@@ -5969,7 +5997,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>165</v>
       </c>
@@ -5983,7 +6011,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>166</v>
       </c>
@@ -5997,7 +6025,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>167</v>
       </c>
@@ -6014,7 +6042,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>168</v>
       </c>
@@ -6031,7 +6059,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>169</v>
       </c>
@@ -6048,7 +6076,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>170</v>
       </c>
@@ -6065,7 +6093,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>171</v>
       </c>
@@ -6082,7 +6110,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>172</v>
       </c>
@@ -6099,7 +6127,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>173</v>
       </c>
@@ -6116,7 +6144,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>174</v>
       </c>
@@ -6133,7 +6161,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>175</v>
       </c>
@@ -6147,7 +6175,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>176</v>
       </c>
@@ -6164,7 +6192,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>177</v>
       </c>
@@ -6181,7 +6209,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>178</v>
       </c>
@@ -6198,7 +6226,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>179</v>
       </c>
@@ -6215,7 +6243,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>180</v>
       </c>
@@ -6232,7 +6260,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>181</v>
       </c>
@@ -6249,7 +6277,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>182</v>
       </c>
@@ -6266,7 +6294,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>183</v>
       </c>
@@ -6283,7 +6311,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>184</v>
       </c>
@@ -6300,7 +6328,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>185</v>
       </c>
@@ -6317,7 +6345,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>186</v>
       </c>
@@ -6334,7 +6362,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>187</v>
       </c>
@@ -6351,7 +6379,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>188</v>
       </c>
@@ -6368,7 +6396,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>189</v>
       </c>
@@ -6385,7 +6413,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>190</v>
       </c>
@@ -6402,7 +6430,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>191</v>
       </c>
@@ -6419,7 +6447,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>192</v>
       </c>
@@ -6436,7 +6464,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>193</v>
       </c>
@@ -6453,7 +6481,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>194</v>
       </c>
@@ -6470,7 +6498,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>195</v>
       </c>
@@ -6487,7 +6515,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>196</v>
       </c>
@@ -6504,7 +6532,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>197</v>
       </c>
@@ -6521,7 +6549,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>198</v>
       </c>
@@ -6538,7 +6566,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>199</v>
       </c>
@@ -6555,7 +6583,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>200</v>
       </c>
@@ -6585,14 +6613,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>318</v>
       </c>
@@ -6605,7 +6633,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>319</v>
       </c>
@@ -6620,7 +6648,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>320</v>
       </c>
@@ -6633,7 +6661,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>321</v>
       </c>
@@ -6646,7 +6674,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>322</v>
       </c>
@@ -6659,7 +6687,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>323</v>
       </c>
@@ -6674,7 +6702,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>324</v>
       </c>
@@ -6689,7 +6717,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>325</v>
       </c>
@@ -6706,7 +6734,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>326</v>
       </c>
@@ -6723,7 +6751,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>327</v>
       </c>
@@ -6740,7 +6768,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>328</v>
       </c>
@@ -6757,7 +6785,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>329</v>
       </c>
@@ -6774,7 +6802,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>330</v>
       </c>
@@ -6791,7 +6819,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>556</v>
       </c>
@@ -6806,7 +6834,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>331</v>
       </c>
@@ -6823,7 +6851,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>332</v>
       </c>
@@ -6840,7 +6868,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>333</v>
       </c>
@@ -6857,7 +6885,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>334</v>
       </c>
@@ -6874,7 +6902,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>335</v>
       </c>
@@ -6891,7 +6919,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>336</v>
       </c>
@@ -6906,7 +6934,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>337</v>
       </c>
@@ -6921,7 +6949,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>338</v>
       </c>
@@ -6938,7 +6966,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>366</v>
       </c>
@@ -6955,7 +6983,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>339</v>
       </c>
@@ -6972,7 +7000,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>340</v>
       </c>
@@ -6987,7 +7015,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>341</v>
       </c>
@@ -7004,7 +7032,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>342</v>
       </c>
@@ -7021,7 +7049,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>343</v>
       </c>
@@ -7038,7 +7066,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>344</v>
       </c>
@@ -7055,7 +7083,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>345</v>
       </c>
@@ -7072,7 +7100,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>346</v>
       </c>
@@ -7089,7 +7117,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>347</v>
       </c>
@@ -7106,7 +7134,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>348</v>
       </c>
@@ -7123,7 +7151,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>349</v>
       </c>
@@ -7140,7 +7168,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>350</v>
       </c>
@@ -7157,7 +7185,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>351</v>
       </c>
@@ -7174,7 +7202,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>352</v>
       </c>
@@ -7191,7 +7219,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>353</v>
       </c>
@@ -7208,7 +7236,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>354</v>
       </c>
@@ -7225,7 +7253,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>355</v>
       </c>
@@ -7242,7 +7270,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>356</v>
       </c>
@@ -7259,7 +7287,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>357</v>
       </c>
@@ -7276,7 +7304,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>358</v>
       </c>
@@ -7293,7 +7321,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>359</v>
       </c>
@@ -7310,7 +7338,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>360</v>
       </c>
@@ -7327,7 +7355,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>361</v>
       </c>
@@ -7344,7 +7372,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>362</v>
       </c>
@@ -7361,7 +7389,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>363</v>
       </c>
@@ -7378,7 +7406,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>364</v>
       </c>
@@ -7395,7 +7423,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>365</v>
       </c>
@@ -7425,14 +7453,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="91" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>237</v>
       </c>
@@ -7445,7 +7473,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>238</v>
       </c>
@@ -7460,7 +7488,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>239</v>
       </c>
@@ -7473,7 +7501,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>286</v>
       </c>
@@ -7486,7 +7514,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>240</v>
       </c>
@@ -7499,7 +7527,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>241</v>
       </c>
@@ -7514,7 +7542,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>242</v>
       </c>
@@ -7529,7 +7557,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>243</v>
       </c>
@@ -7546,7 +7574,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>244</v>
       </c>
@@ -7563,7 +7591,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>245</v>
       </c>
@@ -7580,7 +7608,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>246</v>
       </c>
@@ -7597,7 +7625,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>247</v>
       </c>
@@ -7614,7 +7642,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>248</v>
       </c>
@@ -7631,7 +7659,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>249</v>
       </c>
@@ -7646,7 +7674,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>250</v>
       </c>
@@ -7663,7 +7691,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>251</v>
       </c>
@@ -7680,7 +7708,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>252</v>
       </c>
@@ -7697,7 +7725,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>253</v>
       </c>
@@ -7714,7 +7742,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>254</v>
       </c>
@@ -7731,7 +7759,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>255</v>
       </c>
@@ -7746,7 +7774,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>256</v>
       </c>
@@ -7761,7 +7789,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>287</v>
       </c>
@@ -7778,7 +7806,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>288</v>
       </c>
@@ -7795,7 +7823,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>257</v>
       </c>
@@ -7810,7 +7838,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>258</v>
       </c>
@@ -7827,7 +7855,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>259</v>
       </c>
@@ -7844,7 +7872,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>260</v>
       </c>
@@ -7861,7 +7889,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>261</v>
       </c>
@@ -7878,7 +7906,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>262</v>
       </c>
@@ -7895,7 +7923,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>263</v>
       </c>
@@ -7912,7 +7940,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>264</v>
       </c>
@@ -7929,7 +7957,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>265</v>
       </c>
@@ -7946,7 +7974,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>266</v>
       </c>
@@ -7963,7 +7991,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>267</v>
       </c>
@@ -7980,7 +8008,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>268</v>
       </c>
@@ -7997,7 +8025,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>269</v>
       </c>
@@ -8014,7 +8042,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>270</v>
       </c>
@@ -8031,7 +8059,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>271</v>
       </c>
@@ -8048,7 +8076,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>272</v>
       </c>
@@ -8065,7 +8093,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>273</v>
       </c>
@@ -8082,7 +8110,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>274</v>
       </c>
@@ -8099,7 +8127,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>275</v>
       </c>
@@ -8116,7 +8144,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>276</v>
       </c>
@@ -8133,7 +8161,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>277</v>
       </c>
@@ -8150,7 +8178,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>278</v>
       </c>
@@ -8167,7 +8195,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>279</v>
       </c>
@@ -8184,7 +8212,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>280</v>
       </c>
@@ -8201,7 +8229,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>281</v>
       </c>
@@ -8218,7 +8246,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>282</v>
       </c>
@@ -8248,15 +8276,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>397</v>
       </c>
@@ -8269,7 +8297,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>398</v>
       </c>
@@ -8284,7 +8312,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>399</v>
       </c>
@@ -8297,7 +8325,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>400</v>
       </c>
@@ -8310,7 +8338,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>401</v>
       </c>
@@ -8323,7 +8351,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>402</v>
       </c>
@@ -8338,7 +8366,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>403</v>
       </c>
@@ -8353,7 +8381,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>404</v>
       </c>
@@ -8370,7 +8398,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>405</v>
       </c>
@@ -8387,7 +8415,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>406</v>
       </c>
@@ -8404,7 +8432,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>407</v>
       </c>
@@ -8421,7 +8449,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>408</v>
       </c>
@@ -8438,7 +8466,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>409</v>
       </c>
@@ -8455,7 +8483,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>410</v>
       </c>
@@ -8470,7 +8498,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>411</v>
       </c>
@@ -8487,7 +8515,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>412</v>
       </c>
@@ -8504,7 +8532,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>413</v>
       </c>
@@ -8521,7 +8549,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>414</v>
       </c>
@@ -8538,7 +8566,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>415</v>
       </c>
@@ -8555,7 +8583,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>416</v>
       </c>
@@ -8570,7 +8598,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>417</v>
       </c>
@@ -8585,7 +8613,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>444</v>
       </c>
@@ -8602,7 +8630,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>445</v>
       </c>
@@ -8619,7 +8647,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>418</v>
       </c>
@@ -8634,7 +8662,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>419</v>
       </c>
@@ -8651,7 +8679,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>420</v>
       </c>
@@ -8668,7 +8696,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>421</v>
       </c>
@@ -8685,7 +8713,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>422</v>
       </c>
@@ -8702,7 +8730,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>423</v>
       </c>
@@ -8719,7 +8747,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>424</v>
       </c>
@@ -8736,7 +8764,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>425</v>
       </c>
@@ -8753,7 +8781,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>426</v>
       </c>
@@ -8770,7 +8798,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>427</v>
       </c>
@@ -8787,7 +8815,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>428</v>
       </c>
@@ -8804,7 +8832,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>429</v>
       </c>
@@ -8821,7 +8849,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>430</v>
       </c>
@@ -8838,7 +8866,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>431</v>
       </c>
@@ -8855,7 +8883,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>432</v>
       </c>
@@ -8872,7 +8900,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>433</v>
       </c>
@@ -8889,7 +8917,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>434</v>
       </c>
@@ -8906,7 +8934,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>435</v>
       </c>
@@ -8923,7 +8951,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>436</v>
       </c>
@@ -8940,7 +8968,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>437</v>
       </c>
@@ -8957,7 +8985,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>438</v>
       </c>
@@ -8974,7 +9002,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>439</v>
       </c>
@@ -8991,7 +9019,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>440</v>
       </c>
@@ -9008,7 +9036,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>441</v>
       </c>
@@ -9025,7 +9053,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>442</v>
       </c>
@@ -9042,7 +9070,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>443</v>
       </c>
@@ -9072,11 +9100,11 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="91" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -9895,14 +9923,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>367</v>
       </c>
@@ -9915,7 +9943,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>368</v>
       </c>
@@ -9930,7 +9958,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>369</v>
       </c>
@@ -9943,7 +9971,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>370</v>
       </c>
@@ -9956,7 +9984,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>371</v>
       </c>
@@ -9969,7 +9997,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>372</v>
       </c>
@@ -9984,7 +10012,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>373</v>
       </c>
@@ -9999,7 +10027,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>374</v>
       </c>
@@ -10016,7 +10044,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>375</v>
       </c>
@@ -10033,7 +10061,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>376</v>
       </c>
@@ -10050,7 +10078,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>377</v>
       </c>
@@ -10067,7 +10095,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>378</v>
       </c>
@@ -10084,7 +10112,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>379</v>
       </c>
@@ -10101,7 +10129,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>380</v>
       </c>
@@ -10116,7 +10144,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>381</v>
       </c>
@@ -10133,7 +10161,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>382</v>
       </c>
@@ -10150,7 +10178,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>383</v>
       </c>
@@ -10167,7 +10195,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>384</v>
       </c>
@@ -10184,7 +10212,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>385</v>
       </c>
@@ -10201,7 +10229,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>386</v>
       </c>
@@ -10216,7 +10244,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>387</v>
       </c>
@@ -10231,7 +10259,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>388</v>
       </c>
@@ -10246,7 +10274,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>389</v>
       </c>
@@ -10263,7 +10291,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>390</v>
       </c>
@@ -10280,7 +10308,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>391</v>
       </c>
@@ -10297,7 +10325,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>392</v>
       </c>
@@ -10314,7 +10342,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>393</v>
       </c>
@@ -10331,7 +10359,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>394</v>
       </c>
@@ -10348,7 +10376,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>395</v>
       </c>
@@ -10365,7 +10393,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>396</v>
       </c>
@@ -10395,11 +10423,11 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>